<commit_message>
Updated Input AddFare -> now with decimal places
</commit_message>
<xml_diff>
--- a/log_in.xlsx
+++ b/log_in.xlsx
@@ -680,7 +680,7 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
-        <v>44413.70106576352</v>
+        <v>44413.70106576389</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -708,7 +708,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1007,6 +1007,48 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>44413.71606891204</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test01</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Test10</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1021,7 +1063,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1119,6 +1161,16 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>44413.71625334924</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Test01 Test10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>